<commit_message>
Fase IF e ID (modulo paradas)
Modulo de paradas implementado para fases de instruction fetch e
instruction decode. Simulaciones creadas para ambas fases.
</commit_message>
<xml_diff>
--- a/PDFs/Señales de control.xlsx
+++ b/PDFs/Señales de control.xlsx
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -710,7 +710,7 @@
         <v>36</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>27</v>
@@ -730,7 +730,7 @@
         <v>39</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>28</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="15" spans="3:8">
       <c r="G15" s="8" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>29</v>
@@ -749,7 +749,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="G16" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>30</v>
@@ -771,7 +771,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="G18" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>32</v>
@@ -782,7 +782,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="G19" s="10" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>38</v>

</xml_diff>